<commit_message>
Improve pluginWithState, and add test case for core api
</commit_message>
<xml_diff>
--- a/roosterjs 8.xlsx
+++ b/roosterjs 8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\roosterjs\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5475E30B-7492-46C3-88A2-C72E4F23040D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B0DDF7-7B7C-45FB-9BB3-856FEDA956AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="20880" activeTab="1" xr2:uid="{D28651F8-BDF3-4BEE-B8E5-9A987CC4E961}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="20880" xr2:uid="{D28651F8-BDF3-4BEE-B8E5-9A987CC4E961}"/>
   </bookViews>
   <sheets>
     <sheet name="Add" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="429">
   <si>
     <t>Package</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -504,10 +504,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>EditorCore.allowKeyboardEventPropagation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>EditorCore.corePlugins</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -848,10 +844,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PluginWithViewState&lt;T&gt;.state</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Editor.getContent.triggerContentChangedEvent</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1474,14 +1466,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DOMEventHandlerObject.eventType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DOMEventHandlerObject.handler</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PluginEVentType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1622,7 +1606,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LifecyclePluginState.initialContent</t>
+    <t>LifecyclePluginState.customData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record&lt;string, CustomData&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LifecyclePluginState.defaultFormat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DefaultFormat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOMEventHandlerObject.pluginEventType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOMEventHandlerObject.beforeDispatch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EditorOptions.allowKeyboardEventPropagation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EditorCore.currentUndoSnapshot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1630,43 +1642,87 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LifecyclePluginState.customData</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Record&lt;string, CustomData&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LifecyclePluginState.style</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CSSStyleDeclaration</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LifecyclePluginState.calculatedFormat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string[]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LifecyclePluginState.startPosition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NodePosition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LifecyclePluginState.defaultFormat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DefaultFormat</t>
+    <t>use core.undo.value.outerUndoSnapshot instead</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type.member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttachDomEvent.pluginEventType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttachDomEvent.eventName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttachDomEvent.beforeDispatch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PluginEventType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>use AttachDomEvent.eventMap instead</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttachDomEvent.eventMap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record&lt;string, DOMEventHandler&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PluginWithViewState&lt;T&gt;.getState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AutoCompletePlugin.getState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EditPlugin.getState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOMEventPlugin.getState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LifecyclePlugin.getState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DarkModePlugin.getState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>class.member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UndoPlugin.getState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UndoPluginState.outerUndoSnapshot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2031,10 +2087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8071A7B6-AAB2-483B-89D6-B81D0338F88A}">
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2166,7 +2222,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2177,7 +2233,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D9" t="s">
         <v>26</v>
@@ -2194,7 +2250,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
@@ -2211,7 +2267,7 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D11" t="s">
         <v>26</v>
@@ -2228,7 +2284,7 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
         <v>26</v>
@@ -2267,13 +2323,13 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C15" t="s">
+        <v>356</v>
+      </c>
+      <c r="D15" t="s">
         <v>357</v>
-      </c>
-      <c r="C15" t="s">
-        <v>358</v>
-      </c>
-      <c r="D15" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2281,13 +2337,13 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
+        <v>358</v>
+      </c>
+      <c r="C16" t="s">
+        <v>359</v>
+      </c>
+      <c r="D16" t="s">
         <v>360</v>
-      </c>
-      <c r="C16" t="s">
-        <v>361</v>
-      </c>
-      <c r="D16" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2295,10 +2351,10 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C17" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2306,13 +2362,13 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C18" t="s">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="D18" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2320,13 +2376,13 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C19" t="s">
-        <v>367</v>
+        <v>404</v>
       </c>
       <c r="D19" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2334,10 +2390,10 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C20" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2488,10 +2544,13 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D31" t="s">
-        <v>49</v>
+        <v>131</v>
+      </c>
+      <c r="F31" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2502,13 +2561,13 @@
         <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="D32" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="F32" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2519,13 +2578,10 @@
         <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>148</v>
+        <v>380</v>
       </c>
       <c r="D33" t="s">
-        <v>149</v>
-      </c>
-      <c r="F33" t="s">
-        <v>150</v>
+        <v>381</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -2536,10 +2592,10 @@
         <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>384</v>
+        <v>150</v>
       </c>
       <c r="D34" t="s">
-        <v>385</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2550,10 +2606,10 @@
         <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D35" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -2561,13 +2617,16 @@
         <v>109</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D36" t="s">
-        <v>156</v>
+        <v>49</v>
+      </c>
+      <c r="F36" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2575,16 +2634,13 @@
         <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
-      </c>
-      <c r="F37" t="s">
-        <v>158</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2592,13 +2648,13 @@
         <v>109</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>158</v>
       </c>
       <c r="C38" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2606,13 +2662,13 @@
         <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C39" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D39" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2620,13 +2676,13 @@
         <v>109</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D40" t="s">
-        <v>163</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2634,13 +2690,13 @@
         <v>109</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>158</v>
       </c>
       <c r="C41" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="D41" t="s">
-        <v>96</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2648,13 +2704,13 @@
         <v>109</v>
       </c>
       <c r="B42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
         <v>175</v>
       </c>
       <c r="D42" t="s">
-        <v>161</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2662,13 +2718,13 @@
         <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C43" t="s">
         <v>176</v>
       </c>
       <c r="D43" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -2676,13 +2732,13 @@
         <v>109</v>
       </c>
       <c r="B44" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C44" t="s">
-        <v>177</v>
+        <v>416</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>417</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2693,10 +2749,10 @@
         <v>28</v>
       </c>
       <c r="C45" t="s">
+        <v>182</v>
+      </c>
+      <c r="D45" t="s">
         <v>183</v>
-      </c>
-      <c r="D45" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2704,10 +2760,13 @@
         <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C46" t="s">
-        <v>202</v>
+        <v>405</v>
+      </c>
+      <c r="D46" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2715,13 +2774,10 @@
         <v>109</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>203</v>
-      </c>
-      <c r="D47" t="s">
-        <v>59</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -2729,16 +2785,13 @@
         <v>109</v>
       </c>
       <c r="B48" t="s">
-        <v>219</v>
+        <v>28</v>
       </c>
       <c r="C48" t="s">
-        <v>210</v>
+        <v>418</v>
       </c>
       <c r="D48" t="s">
-        <v>163</v>
-      </c>
-      <c r="E48" t="s">
-        <v>164</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2746,13 +2799,16 @@
         <v>109</v>
       </c>
       <c r="B49" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C49" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D49" t="s">
-        <v>111</v>
+        <v>162</v>
+      </c>
+      <c r="E49" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2760,13 +2816,13 @@
         <v>109</v>
       </c>
       <c r="B50" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C50" t="s">
-        <v>386</v>
+        <v>215</v>
       </c>
       <c r="D50" t="s">
-        <v>387</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2774,13 +2830,13 @@
         <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C51" t="s">
-        <v>228</v>
-      </c>
-      <c r="F51" t="s">
-        <v>229</v>
+        <v>382</v>
+      </c>
+      <c r="D51" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2788,10 +2844,13 @@
         <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="C52" t="s">
-        <v>252</v>
+        <v>226</v>
+      </c>
+      <c r="F52" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2799,13 +2858,13 @@
         <v>109</v>
       </c>
       <c r="B53" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="C53" t="s">
-        <v>254</v>
+        <v>419</v>
       </c>
       <c r="D53" t="s">
-        <v>244</v>
+        <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2813,13 +2872,13 @@
         <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="C54" t="s">
-        <v>255</v>
+        <v>421</v>
       </c>
       <c r="D54" t="s">
-        <v>256</v>
+        <v>420</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2827,13 +2886,10 @@
         <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C55" t="s">
-        <v>257</v>
-      </c>
-      <c r="D55" t="s">
-        <v>22</v>
+        <v>250</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2841,13 +2897,13 @@
         <v>109</v>
       </c>
       <c r="B56" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C56" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D56" t="s">
-        <v>65</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2855,13 +2911,13 @@
         <v>109</v>
       </c>
       <c r="B57" t="s">
-        <v>28</v>
+        <v>251</v>
       </c>
       <c r="C57" t="s">
-        <v>398</v>
+        <v>253</v>
       </c>
       <c r="D57" t="s">
-        <v>380</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2869,13 +2925,13 @@
         <v>109</v>
       </c>
       <c r="B58" t="s">
-        <v>28</v>
+        <v>251</v>
       </c>
       <c r="C58" t="s">
-        <v>399</v>
+        <v>255</v>
       </c>
       <c r="D58" t="s">
-        <v>400</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2886,7 +2942,10 @@
         <v>251</v>
       </c>
       <c r="C59" t="s">
-        <v>261</v>
+        <v>256</v>
+      </c>
+      <c r="D59" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2894,13 +2953,13 @@
         <v>109</v>
       </c>
       <c r="B60" t="s">
-        <v>253</v>
+        <v>28</v>
       </c>
       <c r="C60" t="s">
-        <v>262</v>
+        <v>394</v>
       </c>
       <c r="D60" t="s">
-        <v>244</v>
+        <v>376</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2908,13 +2967,13 @@
         <v>109</v>
       </c>
       <c r="B61" t="s">
-        <v>253</v>
+        <v>28</v>
       </c>
       <c r="C61" t="s">
-        <v>263</v>
+        <v>395</v>
       </c>
       <c r="D61" t="s">
-        <v>246</v>
+        <v>396</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2922,10 +2981,13 @@
         <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="C62" t="s">
-        <v>264</v>
+        <v>422</v>
+      </c>
+      <c r="D62" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2933,13 +2995,10 @@
         <v>109</v>
       </c>
       <c r="B63" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C63" t="s">
-        <v>269</v>
-      </c>
-      <c r="D63" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -2947,13 +3006,13 @@
         <v>109</v>
       </c>
       <c r="B64" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C64" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D64" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2961,10 +3020,10 @@
         <v>109</v>
       </c>
       <c r="B65" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C65" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D65" t="s">
         <v>244</v>
@@ -2975,13 +3034,10 @@
         <v>109</v>
       </c>
       <c r="B66" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C66" t="s">
-        <v>267</v>
-      </c>
-      <c r="D66" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -2989,13 +3045,13 @@
         <v>109</v>
       </c>
       <c r="B67" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D67" t="s">
         <v>268</v>
-      </c>
-      <c r="D67" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -3003,10 +3059,13 @@
         <v>109</v>
       </c>
       <c r="B68" t="s">
-        <v>401</v>
+        <v>251</v>
       </c>
       <c r="C68" t="s">
-        <v>385</v>
+        <v>263</v>
+      </c>
+      <c r="D68" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -3014,10 +3073,13 @@
         <v>109</v>
       </c>
       <c r="B69" t="s">
-        <v>363</v>
+        <v>251</v>
       </c>
       <c r="C69" t="s">
-        <v>402</v>
+        <v>264</v>
+      </c>
+      <c r="D69" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -3025,13 +3087,13 @@
         <v>109</v>
       </c>
       <c r="B70" t="s">
-        <v>365</v>
+        <v>251</v>
       </c>
       <c r="C70" t="s">
-        <v>403</v>
+        <v>265</v>
       </c>
       <c r="D70" t="s">
-        <v>404</v>
+        <v>244</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -3039,13 +3101,13 @@
         <v>109</v>
       </c>
       <c r="B71" t="s">
-        <v>365</v>
+        <v>251</v>
       </c>
       <c r="C71" t="s">
-        <v>405</v>
+        <v>266</v>
       </c>
       <c r="D71" t="s">
-        <v>406</v>
+        <v>244</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -3053,13 +3115,13 @@
         <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>365</v>
+        <v>28</v>
       </c>
       <c r="C72" t="s">
-        <v>407</v>
+        <v>427</v>
       </c>
       <c r="D72" t="s">
-        <v>408</v>
+        <v>428</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -3067,13 +3129,13 @@
         <v>109</v>
       </c>
       <c r="B73" t="s">
-        <v>365</v>
+        <v>425</v>
       </c>
       <c r="C73" t="s">
-        <v>409</v>
+        <v>426</v>
       </c>
       <c r="D73" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -3081,13 +3143,10 @@
         <v>109</v>
       </c>
       <c r="B74" t="s">
-        <v>365</v>
+        <v>397</v>
       </c>
       <c r="C74" t="s">
-        <v>411</v>
-      </c>
-      <c r="D74" t="s">
-        <v>412</v>
+        <v>381</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -3095,66 +3154,66 @@
         <v>109</v>
       </c>
       <c r="B75" t="s">
-        <v>365</v>
+        <v>230</v>
       </c>
       <c r="C75" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="D75" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B76" t="s">
-        <v>251</v>
+        <v>361</v>
       </c>
       <c r="C76" t="s">
-        <v>280</v>
+        <v>398</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B77" t="s">
-        <v>246</v>
+        <v>363</v>
       </c>
       <c r="C77" t="s">
-        <v>281</v>
+        <v>399</v>
       </c>
       <c r="D77" t="s">
-        <v>282</v>
+        <v>400</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B78" t="s">
-        <v>70</v>
+        <v>363</v>
       </c>
       <c r="C78" t="s">
-        <v>283</v>
+        <v>401</v>
       </c>
       <c r="D78" t="s">
-        <v>284</v>
+        <v>402</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B79" t="s">
-        <v>70</v>
+        <v>230</v>
       </c>
       <c r="C79" t="s">
-        <v>285</v>
+        <v>424</v>
       </c>
       <c r="D79" t="s">
-        <v>286</v>
+        <v>420</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -3162,10 +3221,10 @@
         <v>104</v>
       </c>
       <c r="B80" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="C80" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -3173,13 +3232,13 @@
         <v>104</v>
       </c>
       <c r="B81" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C81" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="D81" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -3187,10 +3246,13 @@
         <v>104</v>
       </c>
       <c r="B82" t="s">
-        <v>251</v>
+        <v>70</v>
       </c>
       <c r="C82" t="s">
-        <v>291</v>
+        <v>281</v>
+      </c>
+      <c r="D82" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -3198,13 +3260,13 @@
         <v>104</v>
       </c>
       <c r="B83" t="s">
-        <v>253</v>
+        <v>70</v>
       </c>
       <c r="C83" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="D83" t="s">
-        <v>244</v>
+        <v>284</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -3212,13 +3274,10 @@
         <v>104</v>
       </c>
       <c r="B84" t="s">
-        <v>253</v>
+        <v>285</v>
       </c>
       <c r="C84" t="s">
-        <v>293</v>
-      </c>
-      <c r="D84" t="s">
-        <v>244</v>
+        <v>286</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -3226,10 +3285,13 @@
         <v>104</v>
       </c>
       <c r="B85" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C85" t="s">
-        <v>296</v>
+        <v>287</v>
+      </c>
+      <c r="D85" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -3237,13 +3299,10 @@
         <v>104</v>
       </c>
       <c r="B86" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C86" t="s">
-        <v>297</v>
-      </c>
-      <c r="D86" t="s">
-        <v>244</v>
+        <v>289</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -3251,13 +3310,13 @@
         <v>104</v>
       </c>
       <c r="B87" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C87" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D87" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -3265,13 +3324,13 @@
         <v>104</v>
       </c>
       <c r="B88" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C88" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="D88" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -3279,13 +3338,10 @@
         <v>104</v>
       </c>
       <c r="B89" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C89" t="s">
-        <v>300</v>
-      </c>
-      <c r="D89" t="s">
-        <v>244</v>
+        <v>294</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -3293,13 +3349,13 @@
         <v>104</v>
       </c>
       <c r="B90" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C90" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D90" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -3307,13 +3363,13 @@
         <v>104</v>
       </c>
       <c r="B91" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C91" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="D91" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -3324,7 +3380,10 @@
         <v>251</v>
       </c>
       <c r="C92" t="s">
-        <v>303</v>
+        <v>297</v>
+      </c>
+      <c r="D92" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -3332,13 +3391,13 @@
         <v>104</v>
       </c>
       <c r="B93" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C93" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D93" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -3349,7 +3408,10 @@
         <v>251</v>
       </c>
       <c r="C94" t="s">
-        <v>305</v>
+        <v>299</v>
+      </c>
+      <c r="D94" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -3357,13 +3419,13 @@
         <v>104</v>
       </c>
       <c r="B95" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C95" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="D95" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -3371,13 +3433,10 @@
         <v>104</v>
       </c>
       <c r="B96" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C96" t="s">
-        <v>307</v>
-      </c>
-      <c r="D96" t="s">
-        <v>244</v>
+        <v>301</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -3388,7 +3447,10 @@
         <v>251</v>
       </c>
       <c r="C97" t="s">
-        <v>308</v>
+        <v>302</v>
+      </c>
+      <c r="D97" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -3396,13 +3458,10 @@
         <v>104</v>
       </c>
       <c r="B98" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C98" t="s">
-        <v>309</v>
-      </c>
-      <c r="D98" t="s">
-        <v>244</v>
+        <v>303</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -3410,13 +3469,13 @@
         <v>104</v>
       </c>
       <c r="B99" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C99" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D99" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -3427,7 +3486,10 @@
         <v>251</v>
       </c>
       <c r="C100" t="s">
-        <v>311</v>
+        <v>305</v>
+      </c>
+      <c r="D100" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -3435,13 +3497,10 @@
         <v>104</v>
       </c>
       <c r="B101" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C101" t="s">
-        <v>312</v>
-      </c>
-      <c r="D101" t="s">
-        <v>244</v>
+        <v>306</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -3452,7 +3511,10 @@
         <v>251</v>
       </c>
       <c r="C102" t="s">
-        <v>313</v>
+        <v>307</v>
+      </c>
+      <c r="D102" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -3460,13 +3522,13 @@
         <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C103" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D103" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -3474,10 +3536,10 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C104" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -3485,13 +3547,13 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C105" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D105" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -3499,13 +3561,10 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C106" t="s">
-        <v>317</v>
-      </c>
-      <c r="D106" t="s">
-        <v>244</v>
+        <v>311</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -3513,13 +3572,13 @@
         <v>104</v>
       </c>
       <c r="B107" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C107" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="D107" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -3527,13 +3586,10 @@
         <v>104</v>
       </c>
       <c r="B108" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C108" t="s">
-        <v>319</v>
-      </c>
-      <c r="D108" t="s">
-        <v>244</v>
+        <v>313</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -3544,7 +3600,10 @@
         <v>251</v>
       </c>
       <c r="C109" t="s">
-        <v>320</v>
+        <v>314</v>
+      </c>
+      <c r="D109" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -3552,13 +3611,13 @@
         <v>104</v>
       </c>
       <c r="B110" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C110" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D110" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -3566,13 +3625,13 @@
         <v>104</v>
       </c>
       <c r="B111" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C111" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D111" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -3580,13 +3639,13 @@
         <v>104</v>
       </c>
       <c r="B112" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C112" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D112" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
@@ -3594,13 +3653,10 @@
         <v>104</v>
       </c>
       <c r="B113" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C113" t="s">
-        <v>324</v>
-      </c>
-      <c r="D113" t="s">
-        <v>244</v>
+        <v>318</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -3608,13 +3664,69 @@
         <v>104</v>
       </c>
       <c r="B114" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C114" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D114" t="s">
-        <v>244</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>104</v>
+      </c>
+      <c r="B115" t="s">
+        <v>251</v>
+      </c>
+      <c r="C115" t="s">
+        <v>320</v>
+      </c>
+      <c r="D115" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>104</v>
+      </c>
+      <c r="B116" t="s">
+        <v>251</v>
+      </c>
+      <c r="C116" t="s">
+        <v>321</v>
+      </c>
+      <c r="D116" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>104</v>
+      </c>
+      <c r="B117" t="s">
+        <v>251</v>
+      </c>
+      <c r="C117" t="s">
+        <v>322</v>
+      </c>
+      <c r="D117" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>104</v>
+      </c>
+      <c r="B118" t="s">
+        <v>251</v>
+      </c>
+      <c r="C118" t="s">
+        <v>323</v>
+      </c>
+      <c r="D118" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3626,10 +3738,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE16B634-B0AC-4AD5-8573-08B94DE84278}">
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4165,13 +4277,13 @@
         <v>28</v>
       </c>
       <c r="C35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" t="s">
         <v>118</v>
       </c>
-      <c r="D35" t="s">
+      <c r="F35" t="s">
         <v>119</v>
-      </c>
-      <c r="F35" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -4182,13 +4294,13 @@
         <v>28</v>
       </c>
       <c r="C36" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" t="s">
         <v>121</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F36" t="s">
         <v>122</v>
-      </c>
-      <c r="F36" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -4199,13 +4311,13 @@
         <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D37" t="s">
         <v>49</v>
       </c>
       <c r="F37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -4216,13 +4328,13 @@
         <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D38" t="s">
         <v>47</v>
       </c>
       <c r="F38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -4233,13 +4345,13 @@
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D39" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F39" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -4250,13 +4362,13 @@
         <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D40" t="s">
         <v>43</v>
       </c>
       <c r="F40" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -4267,13 +4379,13 @@
         <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D41" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="F41" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -4284,13 +4396,13 @@
         <v>28</v>
       </c>
       <c r="C42" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D42" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F42" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -4301,13 +4413,13 @@
         <v>28</v>
       </c>
       <c r="C43" t="s">
-        <v>134</v>
+        <v>406</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>407</v>
       </c>
       <c r="F43" t="s">
-        <v>136</v>
+        <v>408</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -4318,13 +4430,13 @@
         <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="D44" t="s">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="F44" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -4335,10 +4447,13 @@
         <v>28</v>
       </c>
       <c r="C45" t="s">
-        <v>382</v>
+        <v>152</v>
       </c>
       <c r="D45" t="s">
-        <v>383</v>
+        <v>67</v>
+      </c>
+      <c r="F45" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -4346,16 +4461,13 @@
         <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C46" t="s">
-        <v>168</v>
+        <v>378</v>
       </c>
       <c r="D46" t="s">
-        <v>49</v>
-      </c>
-      <c r="F46" t="s">
-        <v>154</v>
+        <v>379</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -4363,13 +4475,16 @@
         <v>109</v>
       </c>
       <c r="B47" t="s">
-        <v>159</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D47" t="s">
-        <v>161</v>
+        <v>49</v>
+      </c>
+      <c r="F47" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -4377,13 +4492,13 @@
         <v>109</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C48" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D48" t="s">
-        <v>72</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -4391,13 +4506,13 @@
         <v>109</v>
       </c>
       <c r="B49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C49" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D49" t="s">
-        <v>174</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -4405,13 +4520,13 @@
         <v>109</v>
       </c>
       <c r="B50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C50" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -4419,13 +4534,13 @@
         <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C51" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51" t="s">
         <v>173</v>
-      </c>
-      <c r="D51" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -4433,13 +4548,13 @@
         <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="C52" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D52" t="s">
-        <v>111</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -4450,7 +4565,7 @@
         <v>28</v>
       </c>
       <c r="C53" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D53" t="s">
         <v>111</v>
@@ -4464,13 +4579,10 @@
         <v>28</v>
       </c>
       <c r="C54" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="D54" t="s">
-        <v>193</v>
-      </c>
-      <c r="F54" t="s">
-        <v>194</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -4478,13 +4590,16 @@
         <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C55" t="s">
-        <v>130</v>
+        <v>191</v>
+      </c>
+      <c r="D55" t="s">
+        <v>192</v>
       </c>
       <c r="F55" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -4492,13 +4607,13 @@
         <v>109</v>
       </c>
       <c r="B56" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>196</v>
-      </c>
-      <c r="D56" t="s">
-        <v>51</v>
+        <v>129</v>
+      </c>
+      <c r="F56" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -4509,7 +4624,7 @@
         <v>28</v>
       </c>
       <c r="C57" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D57" t="s">
         <v>51</v>
@@ -4523,7 +4638,7 @@
         <v>28</v>
       </c>
       <c r="C58" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D58" t="s">
         <v>51</v>
@@ -4537,7 +4652,7 @@
         <v>28</v>
       </c>
       <c r="C59" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D59" t="s">
         <v>51</v>
@@ -4551,7 +4666,7 @@
         <v>28</v>
       </c>
       <c r="C60" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D60" t="s">
         <v>51</v>
@@ -4565,7 +4680,7 @@
         <v>28</v>
       </c>
       <c r="C61" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D61" t="s">
         <v>51</v>
@@ -4576,16 +4691,13 @@
         <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>219</v>
+        <v>28</v>
       </c>
       <c r="C62" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D62" t="s">
-        <v>111</v>
-      </c>
-      <c r="F62" t="s">
-        <v>208</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -4593,16 +4705,16 @@
         <v>109</v>
       </c>
       <c r="B63" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C63" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D63" t="s">
         <v>111</v>
       </c>
       <c r="F63" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -4610,13 +4722,13 @@
         <v>109</v>
       </c>
       <c r="B64" t="s">
-        <v>28</v>
+        <v>217</v>
       </c>
       <c r="C64" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D64" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="F64" t="s">
         <v>207</v>
@@ -4630,13 +4742,13 @@
         <v>28</v>
       </c>
       <c r="C65" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="D65" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="F65" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -4644,13 +4756,16 @@
         <v>109</v>
       </c>
       <c r="B66" t="s">
-        <v>219</v>
+        <v>28</v>
       </c>
       <c r="C66" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D66" t="s">
-        <v>221</v>
+        <v>96</v>
+      </c>
+      <c r="F66" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -4658,13 +4773,13 @@
         <v>109</v>
       </c>
       <c r="B67" t="s">
+        <v>217</v>
+      </c>
+      <c r="C67" t="s">
+        <v>218</v>
+      </c>
+      <c r="D67" t="s">
         <v>219</v>
-      </c>
-      <c r="C67" t="s">
-        <v>222</v>
-      </c>
-      <c r="D67" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -4672,16 +4787,13 @@
         <v>109</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
+        <v>217</v>
       </c>
       <c r="C68" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D68" t="s">
-        <v>96</v>
-      </c>
-      <c r="F68" t="s">
-        <v>224</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -4689,13 +4801,16 @@
         <v>109</v>
       </c>
       <c r="B69" t="s">
-        <v>219</v>
+        <v>28</v>
       </c>
       <c r="C69" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D69" t="s">
-        <v>51</v>
+        <v>96</v>
+      </c>
+      <c r="F69" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -4703,13 +4818,13 @@
         <v>109</v>
       </c>
       <c r="B70" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C70" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D70" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -4717,16 +4832,13 @@
         <v>109</v>
       </c>
       <c r="B71" t="s">
-        <v>28</v>
+        <v>217</v>
       </c>
       <c r="C71" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D71" t="s">
-        <v>47</v>
-      </c>
-      <c r="F71" t="s">
-        <v>123</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -4737,13 +4849,13 @@
         <v>28</v>
       </c>
       <c r="C72" t="s">
-        <v>388</v>
+        <v>224</v>
       </c>
       <c r="D72" t="s">
-        <v>389</v>
+        <v>47</v>
       </c>
       <c r="F72" t="s">
-        <v>390</v>
+        <v>122</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -4754,10 +4866,13 @@
         <v>28</v>
       </c>
       <c r="C73" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="D73" t="s">
-        <v>359</v>
+        <v>385</v>
+      </c>
+      <c r="F73" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -4768,10 +4883,10 @@
         <v>28</v>
       </c>
       <c r="C74" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="D74" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -4782,13 +4897,10 @@
         <v>28</v>
       </c>
       <c r="C75" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D75" t="s">
-        <v>394</v>
-      </c>
-      <c r="F75" t="s">
-        <v>395</v>
+        <v>357</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -4796,13 +4908,16 @@
         <v>109</v>
       </c>
       <c r="B76" t="s">
-        <v>232</v>
+        <v>28</v>
       </c>
       <c r="C76" t="s">
-        <v>233</v>
+        <v>389</v>
       </c>
       <c r="D76" t="s">
-        <v>51</v>
+        <v>390</v>
+      </c>
+      <c r="F76" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -4810,10 +4925,10 @@
         <v>109</v>
       </c>
       <c r="B77" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C77" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D77" t="s">
         <v>51</v>
@@ -4824,10 +4939,10 @@
         <v>109</v>
       </c>
       <c r="B78" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C78" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D78" t="s">
         <v>51</v>
@@ -4838,33 +4953,30 @@
         <v>109</v>
       </c>
       <c r="B79" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C79" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D79" t="s">
         <v>51</v>
       </c>
-      <c r="F79" t="s">
-        <v>240</v>
-      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>109</v>
       </c>
       <c r="B80" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C80" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D80" t="s">
         <v>51</v>
       </c>
       <c r="F80" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -4872,16 +4984,16 @@
         <v>109</v>
       </c>
       <c r="B81" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C81" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D81" t="s">
         <v>51</v>
       </c>
       <c r="F81" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -4889,27 +5001,30 @@
         <v>109</v>
       </c>
       <c r="B82" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C82" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D82" t="s">
         <v>51</v>
       </c>
+      <c r="F82" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>109</v>
       </c>
       <c r="B83" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C83" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D83" t="s">
-        <v>246</v>
+        <v>51</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -4917,13 +5032,13 @@
         <v>109</v>
       </c>
       <c r="B84" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C84" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D84" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -4931,13 +5046,13 @@
         <v>109</v>
       </c>
       <c r="B85" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C85" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D85" t="s">
-        <v>51</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -4945,10 +5060,10 @@
         <v>109</v>
       </c>
       <c r="B86" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C86" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D86" t="s">
         <v>51</v>
@@ -4959,66 +5074,78 @@
         <v>109</v>
       </c>
       <c r="B87" t="s">
-        <v>357</v>
+        <v>230</v>
       </c>
       <c r="C87" t="s">
-        <v>370</v>
-      </c>
-      <c r="F87" t="s">
-        <v>371</v>
+        <v>248</v>
+      </c>
+      <c r="D87" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>278</v>
+        <v>355</v>
       </c>
       <c r="C88" t="s">
-        <v>327</v>
+        <v>366</v>
       </c>
       <c r="F88" t="s">
-        <v>279</v>
+        <v>367</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B89" t="s">
-        <v>326</v>
+        <v>409</v>
       </c>
       <c r="C89" t="s">
-        <v>328</v>
+        <v>411</v>
+      </c>
+      <c r="D89" t="s">
+        <v>407</v>
+      </c>
+      <c r="F89" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B90" t="s">
-        <v>329</v>
+        <v>409</v>
       </c>
       <c r="C90" t="s">
-        <v>330</v>
+        <v>410</v>
       </c>
       <c r="D90" t="s">
-        <v>331</v>
+        <v>413</v>
+      </c>
+      <c r="F90" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B91" t="s">
-        <v>329</v>
+        <v>409</v>
       </c>
       <c r="C91" t="s">
-        <v>332</v>
+        <v>412</v>
       </c>
       <c r="D91" t="s">
-        <v>333</v>
+        <v>414</v>
+      </c>
+      <c r="F91" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -5026,16 +5153,13 @@
         <v>104</v>
       </c>
       <c r="B92" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
       <c r="C92" t="s">
-        <v>334</v>
-      </c>
-      <c r="D92" t="s">
-        <v>234</v>
+        <v>325</v>
       </c>
       <c r="F92" t="s">
-        <v>341</v>
+        <v>277</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -5043,13 +5167,10 @@
         <v>104</v>
       </c>
       <c r="B93" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C93" t="s">
-        <v>337</v>
-      </c>
-      <c r="D93" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -5057,16 +5178,13 @@
         <v>104</v>
       </c>
       <c r="B94" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C94" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="D94" t="s">
-        <v>234</v>
-      </c>
-      <c r="F94" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -5074,13 +5192,13 @@
         <v>104</v>
       </c>
       <c r="B95" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C95" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="D95" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -5088,16 +5206,16 @@
         <v>104</v>
       </c>
       <c r="B96" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C96" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D96" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F96" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -5105,13 +5223,13 @@
         <v>104</v>
       </c>
       <c r="B97" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C97" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D97" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -5119,16 +5237,16 @@
         <v>104</v>
       </c>
       <c r="B98" t="s">
-        <v>246</v>
+        <v>324</v>
       </c>
       <c r="C98" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="D98" t="s">
-        <v>345</v>
+        <v>232</v>
       </c>
       <c r="F98" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -5136,13 +5254,13 @@
         <v>104</v>
       </c>
       <c r="B99" t="s">
-        <v>70</v>
+        <v>327</v>
       </c>
       <c r="C99" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="D99" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -5150,13 +5268,16 @@
         <v>104</v>
       </c>
       <c r="B100" t="s">
-        <v>70</v>
+        <v>324</v>
       </c>
       <c r="C100" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="D100" t="s">
-        <v>351</v>
+        <v>232</v>
+      </c>
+      <c r="F100" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -5164,13 +5285,13 @@
         <v>104</v>
       </c>
       <c r="B101" t="s">
-        <v>70</v>
+        <v>327</v>
       </c>
       <c r="C101" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="D101" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -5178,16 +5299,16 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C102" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="D102" t="s">
-        <v>65</v>
+        <v>343</v>
       </c>
       <c r="F102" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -5198,10 +5319,10 @@
         <v>70</v>
       </c>
       <c r="C103" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="D103" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -5212,10 +5333,69 @@
         <v>70</v>
       </c>
       <c r="C104" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="D104" t="s">
-        <v>356</v>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>70</v>
+      </c>
+      <c r="C105" t="s">
+        <v>347</v>
+      </c>
+      <c r="D105" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>244</v>
+      </c>
+      <c r="C106" t="s">
+        <v>350</v>
+      </c>
+      <c r="D106" t="s">
+        <v>65</v>
+      </c>
+      <c r="F106" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>104</v>
+      </c>
+      <c r="B107" t="s">
+        <v>70</v>
+      </c>
+      <c r="C107" t="s">
+        <v>352</v>
+      </c>
+      <c r="D107" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>104</v>
+      </c>
+      <c r="B108" t="s">
+        <v>70</v>
+      </c>
+      <c r="C108" t="s">
+        <v>353</v>
+      </c>
+      <c r="D108" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -5366,13 +5546,13 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" t="s">
         <v>128</v>
       </c>
-      <c r="D7" t="s">
+      <c r="H7" t="s">
         <v>129</v>
-      </c>
-      <c r="H7" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -5383,16 +5563,16 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" t="s">
         <v>137</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>138</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>139</v>
-      </c>
-      <c r="H8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -5403,16 +5583,16 @@
         <v>28</v>
       </c>
       <c r="C9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" t="s">
         <v>141</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>142</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>143</v>
-      </c>
-      <c r="H9" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -5423,13 +5603,13 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" t="s">
         <v>145</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" t="s">
         <v>146</v>
-      </c>
-      <c r="G10" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -5440,16 +5620,16 @@
         <v>28</v>
       </c>
       <c r="C11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" t="s">
         <v>178</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
         <v>179</v>
       </c>
-      <c r="G11" t="s">
-        <v>180</v>
-      </c>
       <c r="H11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -5460,13 +5640,13 @@
         <v>28</v>
       </c>
       <c r="C12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" t="s">
         <v>185</v>
       </c>
-      <c r="D12" t="s">
-        <v>186</v>
-      </c>
       <c r="G12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -5477,16 +5657,16 @@
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
+        <v>186</v>
+      </c>
+      <c r="G13" t="s">
         <v>187</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>188</v>
-      </c>
-      <c r="H13" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -5494,16 +5674,16 @@
         <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D14" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="H14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -5511,16 +5691,16 @@
         <v>109</v>
       </c>
       <c r="B15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D15" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="H15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -5528,13 +5708,13 @@
         <v>109</v>
       </c>
       <c r="B16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -5542,10 +5722,10 @@
         <v>109</v>
       </c>
       <c r="B17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F17" t="s">
         <v>104</v>
@@ -5556,27 +5736,27 @@
         <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C18" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G18" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>269</v>
+      </c>
+      <c r="B19" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" t="s">
+        <v>270</v>
+      </c>
+      <c r="D19" t="s">
         <v>271</v>
-      </c>
-      <c r="B19" t="s">
-        <v>246</v>
-      </c>
-      <c r="C19" t="s">
-        <v>272</v>
-      </c>
-      <c r="D19" t="s">
-        <v>273</v>
       </c>
       <c r="F19" t="s">
         <v>104</v>
@@ -5584,36 +5764,36 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B20" t="s">
+        <v>272</v>
+      </c>
+      <c r="C20" t="s">
+        <v>273</v>
+      </c>
+      <c r="D20" t="s">
         <v>274</v>
       </c>
-      <c r="C20" t="s">
+      <c r="F20" t="s">
+        <v>104</v>
+      </c>
+      <c r="H20" t="s">
         <v>275</v>
-      </c>
-      <c r="D20" t="s">
-        <v>276</v>
-      </c>
-      <c r="F20" t="s">
-        <v>104</v>
-      </c>
-      <c r="H20" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B21" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G21" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the xlsx file
</commit_message>
<xml_diff>
--- a/roosterjs 8.xlsx
+++ b/roosterjs 8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\roosterjs\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B0DDF7-7B7C-45FB-9BB3-856FEDA956AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADFE8BB-6EC1-40E9-85BB-138D37A63F8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="20880" xr2:uid="{D28651F8-BDF3-4BEE-B8E5-9A987CC4E961}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="437">
   <si>
     <t>Package</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1723,6 +1723,38 @@
   </si>
   <si>
     <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>funciton.param</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function.param</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>readFile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>readFile.file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>readFile.callback</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>void</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>File</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2087,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8071A7B6-AAB2-483B-89D6-B81D0338F88A}">
-  <dimension ref="A1:F118"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2346,7 +2378,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2357,7 +2389,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -2371,7 +2403,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -2385,7 +2417,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2396,7 +2428,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -2410,7 +2442,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -2424,7 +2456,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -2438,7 +2470,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -2452,7 +2484,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -2466,7 +2498,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2480,7 +2512,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -2494,7 +2526,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -2508,52 +2540,49 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>429</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>432</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>430</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>433</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>431</v>
       </c>
       <c r="C31" t="s">
-        <v>130</v>
+        <v>434</v>
       </c>
       <c r="D31" t="s">
-        <v>131</v>
-      </c>
-      <c r="F31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>109</v>
       </c>
@@ -2561,13 +2590,10 @@
         <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>148</v>
-      </c>
-      <c r="F32" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2578,10 +2604,10 @@
         <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>380</v>
+        <v>116</v>
       </c>
       <c r="D33" t="s">
-        <v>381</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -2592,10 +2618,13 @@
         <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D34" t="s">
-        <v>151</v>
+        <v>131</v>
+      </c>
+      <c r="F34" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2606,10 +2635,13 @@
         <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D35" t="s">
-        <v>155</v>
+        <v>148</v>
+      </c>
+      <c r="F35" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -2617,16 +2649,13 @@
         <v>109</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>156</v>
+        <v>380</v>
       </c>
       <c r="D36" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" t="s">
-        <v>157</v>
+        <v>381</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2634,13 +2663,13 @@
         <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" t="s">
         <v>151</v>
-      </c>
-      <c r="D37" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2648,13 +2677,13 @@
         <v>109</v>
       </c>
       <c r="B38" t="s">
-        <v>158</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D38" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2662,13 +2691,16 @@
         <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C39" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D39" t="s">
-        <v>162</v>
+        <v>49</v>
+      </c>
+      <c r="F39" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2679,10 +2711,10 @@
         <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D40" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2693,7 +2725,7 @@
         <v>158</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="D41" t="s">
         <v>160</v>
@@ -2707,10 +2739,10 @@
         <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="D42" t="s">
-        <v>27</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2718,13 +2750,13 @@
         <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>158</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="D43" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -2735,10 +2767,10 @@
         <v>158</v>
       </c>
       <c r="C44" t="s">
-        <v>416</v>
+        <v>174</v>
       </c>
       <c r="D44" t="s">
-        <v>417</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2746,13 +2778,13 @@
         <v>109</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="C45" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D45" t="s">
-        <v>183</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2760,10 +2792,10 @@
         <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="C46" t="s">
-        <v>405</v>
+        <v>176</v>
       </c>
       <c r="D46" t="s">
         <v>49</v>
@@ -2774,10 +2806,13 @@
         <v>109</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="C47" t="s">
-        <v>201</v>
+        <v>416</v>
+      </c>
+      <c r="D47" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -2788,10 +2823,10 @@
         <v>28</v>
       </c>
       <c r="C48" t="s">
-        <v>418</v>
+        <v>182</v>
       </c>
       <c r="D48" t="s">
-        <v>51</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2799,16 +2834,13 @@
         <v>109</v>
       </c>
       <c r="B49" t="s">
-        <v>217</v>
+        <v>28</v>
       </c>
       <c r="C49" t="s">
-        <v>208</v>
+        <v>405</v>
       </c>
       <c r="D49" t="s">
-        <v>162</v>
-      </c>
-      <c r="E49" t="s">
-        <v>163</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2816,13 +2848,10 @@
         <v>109</v>
       </c>
       <c r="B50" t="s">
-        <v>217</v>
+        <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>215</v>
-      </c>
-      <c r="D50" t="s">
-        <v>111</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2830,13 +2859,13 @@
         <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>217</v>
+        <v>28</v>
       </c>
       <c r="C51" t="s">
-        <v>382</v>
+        <v>418</v>
       </c>
       <c r="D51" t="s">
-        <v>383</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2844,13 +2873,16 @@
         <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C52" t="s">
-        <v>226</v>
-      </c>
-      <c r="F52" t="s">
-        <v>227</v>
+        <v>208</v>
+      </c>
+      <c r="D52" t="s">
+        <v>162</v>
+      </c>
+      <c r="E52" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2858,13 +2890,13 @@
         <v>109</v>
       </c>
       <c r="B53" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="C53" t="s">
-        <v>419</v>
+        <v>215</v>
       </c>
       <c r="D53" t="s">
-        <v>420</v>
+        <v>111</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2872,13 +2904,13 @@
         <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="C54" t="s">
-        <v>421</v>
+        <v>382</v>
       </c>
       <c r="D54" t="s">
-        <v>420</v>
+        <v>383</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2886,10 +2918,13 @@
         <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="C55" t="s">
-        <v>250</v>
+        <v>226</v>
+      </c>
+      <c r="F55" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2897,13 +2932,13 @@
         <v>109</v>
       </c>
       <c r="B56" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="C56" t="s">
-        <v>252</v>
+        <v>419</v>
       </c>
       <c r="D56" t="s">
-        <v>242</v>
+        <v>420</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2911,13 +2946,13 @@
         <v>109</v>
       </c>
       <c r="B57" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="C57" t="s">
-        <v>253</v>
+        <v>421</v>
       </c>
       <c r="D57" t="s">
-        <v>254</v>
+        <v>420</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2925,13 +2960,10 @@
         <v>109</v>
       </c>
       <c r="B58" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C58" t="s">
-        <v>255</v>
-      </c>
-      <c r="D58" t="s">
-        <v>22</v>
+        <v>250</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2942,10 +2974,10 @@
         <v>251</v>
       </c>
       <c r="C59" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D59" t="s">
-        <v>65</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2953,13 +2985,13 @@
         <v>109</v>
       </c>
       <c r="B60" t="s">
-        <v>28</v>
+        <v>251</v>
       </c>
       <c r="C60" t="s">
-        <v>394</v>
+        <v>253</v>
       </c>
       <c r="D60" t="s">
-        <v>376</v>
+        <v>254</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2967,13 +2999,13 @@
         <v>109</v>
       </c>
       <c r="B61" t="s">
-        <v>28</v>
+        <v>251</v>
       </c>
       <c r="C61" t="s">
-        <v>395</v>
+        <v>255</v>
       </c>
       <c r="D61" t="s">
-        <v>396</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -2981,13 +3013,13 @@
         <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>230</v>
+        <v>251</v>
       </c>
       <c r="C62" t="s">
-        <v>422</v>
+        <v>256</v>
       </c>
       <c r="D62" t="s">
-        <v>420</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2995,10 +3027,13 @@
         <v>109</v>
       </c>
       <c r="B63" t="s">
-        <v>249</v>
+        <v>28</v>
       </c>
       <c r="C63" t="s">
-        <v>259</v>
+        <v>394</v>
+      </c>
+      <c r="D63" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -3006,13 +3041,13 @@
         <v>109</v>
       </c>
       <c r="B64" t="s">
-        <v>251</v>
+        <v>28</v>
       </c>
       <c r="C64" t="s">
-        <v>260</v>
+        <v>395</v>
       </c>
       <c r="D64" t="s">
-        <v>242</v>
+        <v>396</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -3020,13 +3055,13 @@
         <v>109</v>
       </c>
       <c r="B65" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="C65" t="s">
-        <v>261</v>
+        <v>422</v>
       </c>
       <c r="D65" t="s">
-        <v>244</v>
+        <v>420</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -3037,7 +3072,7 @@
         <v>249</v>
       </c>
       <c r="C66" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -3048,10 +3083,10 @@
         <v>251</v>
       </c>
       <c r="C67" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D67" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -3062,10 +3097,10 @@
         <v>251</v>
       </c>
       <c r="C68" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D68" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -3073,13 +3108,10 @@
         <v>109</v>
       </c>
       <c r="B69" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C69" t="s">
-        <v>264</v>
-      </c>
-      <c r="D69" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -3090,10 +3122,10 @@
         <v>251</v>
       </c>
       <c r="C70" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D70" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -3104,10 +3136,10 @@
         <v>251</v>
       </c>
       <c r="C71" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D71" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -3115,13 +3147,13 @@
         <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>28</v>
+        <v>251</v>
       </c>
       <c r="C72" t="s">
-        <v>427</v>
+        <v>264</v>
       </c>
       <c r="D72" t="s">
-        <v>428</v>
+        <v>242</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -3129,13 +3161,13 @@
         <v>109</v>
       </c>
       <c r="B73" t="s">
-        <v>425</v>
+        <v>251</v>
       </c>
       <c r="C73" t="s">
-        <v>426</v>
+        <v>265</v>
       </c>
       <c r="D73" t="s">
-        <v>420</v>
+        <v>244</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -3143,10 +3175,13 @@
         <v>109</v>
       </c>
       <c r="B74" t="s">
-        <v>397</v>
+        <v>251</v>
       </c>
       <c r="C74" t="s">
-        <v>381</v>
+        <v>266</v>
+      </c>
+      <c r="D74" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -3154,13 +3189,13 @@
         <v>109</v>
       </c>
       <c r="B75" t="s">
-        <v>230</v>
+        <v>28</v>
       </c>
       <c r="C75" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="D75" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -3168,10 +3203,13 @@
         <v>109</v>
       </c>
       <c r="B76" t="s">
-        <v>361</v>
+        <v>425</v>
       </c>
       <c r="C76" t="s">
-        <v>398</v>
+        <v>426</v>
+      </c>
+      <c r="D76" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -3179,13 +3217,10 @@
         <v>109</v>
       </c>
       <c r="B77" t="s">
-        <v>363</v>
+        <v>397</v>
       </c>
       <c r="C77" t="s">
-        <v>399</v>
-      </c>
-      <c r="D77" t="s">
-        <v>400</v>
+        <v>381</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -3193,13 +3228,13 @@
         <v>109</v>
       </c>
       <c r="B78" t="s">
-        <v>363</v>
+        <v>230</v>
       </c>
       <c r="C78" t="s">
-        <v>401</v>
+        <v>423</v>
       </c>
       <c r="D78" t="s">
-        <v>402</v>
+        <v>420</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -3207,52 +3242,52 @@
         <v>109</v>
       </c>
       <c r="B79" t="s">
-        <v>230</v>
+        <v>361</v>
       </c>
       <c r="C79" t="s">
-        <v>424</v>
-      </c>
-      <c r="D79" t="s">
-        <v>420</v>
+        <v>398</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B80" t="s">
-        <v>249</v>
+        <v>363</v>
       </c>
       <c r="C80" t="s">
-        <v>278</v>
+        <v>399</v>
+      </c>
+      <c r="D80" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B81" t="s">
-        <v>244</v>
+        <v>363</v>
       </c>
       <c r="C81" t="s">
-        <v>279</v>
+        <v>401</v>
       </c>
       <c r="D81" t="s">
-        <v>280</v>
+        <v>402</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B82" t="s">
-        <v>70</v>
+        <v>230</v>
       </c>
       <c r="C82" t="s">
-        <v>281</v>
+        <v>424</v>
       </c>
       <c r="D82" t="s">
-        <v>282</v>
+        <v>420</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -3260,13 +3295,10 @@
         <v>104</v>
       </c>
       <c r="B83" t="s">
-        <v>70</v>
+        <v>249</v>
       </c>
       <c r="C83" t="s">
-        <v>283</v>
-      </c>
-      <c r="D83" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -3274,10 +3306,13 @@
         <v>104</v>
       </c>
       <c r="B84" t="s">
-        <v>285</v>
+        <v>244</v>
       </c>
       <c r="C84" t="s">
-        <v>286</v>
+        <v>279</v>
+      </c>
+      <c r="D84" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -3285,13 +3320,13 @@
         <v>104</v>
       </c>
       <c r="B85" t="s">
-        <v>244</v>
+        <v>70</v>
       </c>
       <c r="C85" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D85" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -3299,10 +3334,13 @@
         <v>104</v>
       </c>
       <c r="B86" t="s">
-        <v>249</v>
+        <v>70</v>
       </c>
       <c r="C86" t="s">
-        <v>289</v>
+        <v>283</v>
+      </c>
+      <c r="D86" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -3310,13 +3348,10 @@
         <v>104</v>
       </c>
       <c r="B87" t="s">
-        <v>251</v>
+        <v>285</v>
       </c>
       <c r="C87" t="s">
-        <v>290</v>
-      </c>
-      <c r="D87" t="s">
-        <v>242</v>
+        <v>286</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -3324,13 +3359,13 @@
         <v>104</v>
       </c>
       <c r="B88" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C88" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D88" t="s">
-        <v>242</v>
+        <v>288</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -3341,7 +3376,7 @@
         <v>249</v>
       </c>
       <c r="C89" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -3352,7 +3387,7 @@
         <v>251</v>
       </c>
       <c r="C90" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D90" t="s">
         <v>242</v>
@@ -3366,7 +3401,7 @@
         <v>251</v>
       </c>
       <c r="C91" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D91" t="s">
         <v>242</v>
@@ -3377,13 +3412,10 @@
         <v>104</v>
       </c>
       <c r="B92" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C92" t="s">
-        <v>297</v>
-      </c>
-      <c r="D92" t="s">
-        <v>242</v>
+        <v>294</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -3394,7 +3426,7 @@
         <v>251</v>
       </c>
       <c r="C93" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D93" t="s">
         <v>242</v>
@@ -3408,7 +3440,7 @@
         <v>251</v>
       </c>
       <c r="C94" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D94" t="s">
         <v>242</v>
@@ -3422,7 +3454,7 @@
         <v>251</v>
       </c>
       <c r="C95" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D95" t="s">
         <v>242</v>
@@ -3433,10 +3465,13 @@
         <v>104</v>
       </c>
       <c r="B96" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C96" t="s">
-        <v>301</v>
+        <v>298</v>
+      </c>
+      <c r="D96" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -3447,7 +3482,7 @@
         <v>251</v>
       </c>
       <c r="C97" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D97" t="s">
         <v>242</v>
@@ -3458,10 +3493,13 @@
         <v>104</v>
       </c>
       <c r="B98" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C98" t="s">
-        <v>303</v>
+        <v>300</v>
+      </c>
+      <c r="D98" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -3469,13 +3507,10 @@
         <v>104</v>
       </c>
       <c r="B99" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C99" t="s">
-        <v>304</v>
-      </c>
-      <c r="D99" t="s">
-        <v>242</v>
+        <v>301</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -3486,7 +3521,7 @@
         <v>251</v>
       </c>
       <c r="C100" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D100" t="s">
         <v>242</v>
@@ -3500,7 +3535,7 @@
         <v>249</v>
       </c>
       <c r="C101" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -3511,7 +3546,7 @@
         <v>251</v>
       </c>
       <c r="C102" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D102" t="s">
         <v>242</v>
@@ -3525,7 +3560,7 @@
         <v>251</v>
       </c>
       <c r="C103" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D103" t="s">
         <v>242</v>
@@ -3539,7 +3574,7 @@
         <v>249</v>
       </c>
       <c r="C104" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -3550,7 +3585,7 @@
         <v>251</v>
       </c>
       <c r="C105" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D105" t="s">
         <v>242</v>
@@ -3561,10 +3596,13 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C106" t="s">
-        <v>311</v>
+        <v>308</v>
+      </c>
+      <c r="D106" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -3572,13 +3610,10 @@
         <v>104</v>
       </c>
       <c r="B107" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C107" t="s">
-        <v>312</v>
-      </c>
-      <c r="D107" t="s">
-        <v>242</v>
+        <v>309</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -3586,10 +3621,13 @@
         <v>104</v>
       </c>
       <c r="B108" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C108" t="s">
-        <v>313</v>
+        <v>310</v>
+      </c>
+      <c r="D108" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -3597,13 +3635,10 @@
         <v>104</v>
       </c>
       <c r="B109" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C109" t="s">
-        <v>314</v>
-      </c>
-      <c r="D109" t="s">
-        <v>242</v>
+        <v>311</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -3614,7 +3649,7 @@
         <v>251</v>
       </c>
       <c r="C110" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D110" t="s">
         <v>242</v>
@@ -3625,13 +3660,10 @@
         <v>104</v>
       </c>
       <c r="B111" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C111" t="s">
-        <v>316</v>
-      </c>
-      <c r="D111" t="s">
-        <v>242</v>
+        <v>313</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -3642,7 +3674,7 @@
         <v>251</v>
       </c>
       <c r="C112" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D112" t="s">
         <v>242</v>
@@ -3653,10 +3685,13 @@
         <v>104</v>
       </c>
       <c r="B113" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C113" t="s">
-        <v>318</v>
+        <v>315</v>
+      </c>
+      <c r="D113" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -3667,7 +3702,7 @@
         <v>251</v>
       </c>
       <c r="C114" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D114" t="s">
         <v>242</v>
@@ -3681,7 +3716,7 @@
         <v>251</v>
       </c>
       <c r="C115" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D115" t="s">
         <v>242</v>
@@ -3692,13 +3727,10 @@
         <v>104</v>
       </c>
       <c r="B116" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C116" t="s">
-        <v>321</v>
-      </c>
-      <c r="D116" t="s">
-        <v>242</v>
+        <v>318</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -3709,7 +3741,7 @@
         <v>251</v>
       </c>
       <c r="C117" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D117" t="s">
         <v>242</v>
@@ -3723,9 +3755,51 @@
         <v>251</v>
       </c>
       <c r="C118" t="s">
+        <v>320</v>
+      </c>
+      <c r="D118" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>104</v>
+      </c>
+      <c r="B119" t="s">
+        <v>251</v>
+      </c>
+      <c r="C119" t="s">
+        <v>321</v>
+      </c>
+      <c r="D119" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>104</v>
+      </c>
+      <c r="B120" t="s">
+        <v>251</v>
+      </c>
+      <c r="C120" t="s">
+        <v>322</v>
+      </c>
+      <c r="D120" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>104</v>
+      </c>
+      <c r="B121" t="s">
+        <v>251</v>
+      </c>
+      <c r="C121" t="s">
         <v>323</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D121" t="s">
         <v>242</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update the change file
</commit_message>
<xml_diff>
--- a/roosterjs 8.xlsx
+++ b/roosterjs 8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\roosterjs\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADFE8BB-6EC1-40E9-85BB-138D37A63F8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550C4F46-A898-4539-B0CA-884A96C4F501}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="20880" xr2:uid="{D28651F8-BDF3-4BEE-B8E5-9A987CC4E961}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="447">
   <si>
     <t>Package</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -664,10 +664,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>replace Editor.performAutoComplete API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>type.param</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1048,18 +1044,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DOMEventPluginState.pendableFormatState</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PendableFormatState</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DOMEventPluginState.pendableFormatPosition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DOMEventPluginState.scrollContainer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1755,6 +1743,58 @@
   </si>
   <si>
     <t>File</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PendingFormatStatePluginState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PendingFormatStatePluginState.pendableFormatState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PendingFormatStatePluginState.pendableFormatPosition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CorePlugins.pendingFormatState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CorePlugins.mouseUp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MouseUpPlugin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PendingFormatStatePlugin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Splitted from DOMEventPlugin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Replace Editor.performAutoComplete API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>class.member</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PendingFormatStatePlugin.getState</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2119,10 +2159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8071A7B6-AAB2-483B-89D6-B81D0338F88A}">
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2254,7 +2294,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2265,7 +2305,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D9" t="s">
         <v>26</v>
@@ -2282,7 +2322,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
@@ -2299,7 +2339,7 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D11" t="s">
         <v>26</v>
@@ -2316,7 +2356,7 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D12" t="s">
         <v>26</v>
@@ -2355,13 +2395,13 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C15" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D15" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2369,13 +2409,13 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C16" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D16" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2383,10 +2423,10 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C17" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2394,13 +2434,13 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C18" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D18" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2408,13 +2448,13 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C19" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D19" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2422,10 +2462,10 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C20" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2545,13 +2585,13 @@
         <v>61</v>
       </c>
       <c r="B29" t="s">
+        <v>426</v>
+      </c>
+      <c r="C29" t="s">
         <v>429</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>432</v>
-      </c>
-      <c r="D29" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2559,13 +2599,13 @@
         <v>61</v>
       </c>
       <c r="B30" t="s">
+        <v>427</v>
+      </c>
+      <c r="C30" t="s">
         <v>430</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>433</v>
-      </c>
-      <c r="D30" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2573,13 +2613,13 @@
         <v>61</v>
       </c>
       <c r="B31" t="s">
+        <v>428</v>
+      </c>
+      <c r="C31" t="s">
         <v>431</v>
       </c>
-      <c r="C31" t="s">
-        <v>434</v>
-      </c>
       <c r="D31" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2652,10 +2692,10 @@
         <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D36" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2666,10 +2706,13 @@
         <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>150</v>
+        <v>438</v>
       </c>
       <c r="D37" t="s">
-        <v>151</v>
+        <v>441</v>
+      </c>
+      <c r="F37" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2680,10 +2723,13 @@
         <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>154</v>
+        <v>439</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>440</v>
+      </c>
+      <c r="F38" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2691,16 +2737,13 @@
         <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D39" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2708,13 +2751,13 @@
         <v>109</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D40" t="s">
-        <v>27</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2722,13 +2765,16 @@
         <v>109</v>
       </c>
       <c r="B41" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
       <c r="C41" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D41" t="s">
-        <v>160</v>
+        <v>49</v>
+      </c>
+      <c r="F41" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2736,13 +2782,13 @@
         <v>109</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>30</v>
       </c>
       <c r="C42" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D42" t="s">
-        <v>162</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2750,13 +2796,13 @@
         <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="C43" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D43" t="s">
-        <v>96</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -2764,13 +2810,13 @@
         <v>109</v>
       </c>
       <c r="B44" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C44" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="D44" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2778,13 +2824,13 @@
         <v>109</v>
       </c>
       <c r="B45" t="s">
-        <v>158</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2792,13 +2838,13 @@
         <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C46" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D46" t="s">
-        <v>49</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2806,13 +2852,13 @@
         <v>109</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C47" t="s">
-        <v>416</v>
+        <v>174</v>
       </c>
       <c r="D47" t="s">
-        <v>417</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -2820,13 +2866,13 @@
         <v>109</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
       <c r="C48" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D48" t="s">
-        <v>183</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -2834,13 +2880,13 @@
         <v>109</v>
       </c>
       <c r="B49" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
       <c r="C49" t="s">
-        <v>405</v>
+        <v>413</v>
       </c>
       <c r="D49" t="s">
-        <v>49</v>
+        <v>414</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -2848,10 +2894,13 @@
         <v>109</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C50" t="s">
-        <v>201</v>
+        <v>181</v>
+      </c>
+      <c r="D50" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -2862,10 +2911,10 @@
         <v>28</v>
       </c>
       <c r="C51" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="D51" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -2873,16 +2922,10 @@
         <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>217</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>208</v>
-      </c>
-      <c r="D52" t="s">
-        <v>162</v>
-      </c>
-      <c r="E52" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2890,13 +2933,13 @@
         <v>109</v>
       </c>
       <c r="B53" t="s">
-        <v>217</v>
+        <v>28</v>
       </c>
       <c r="C53" t="s">
-        <v>215</v>
+        <v>415</v>
       </c>
       <c r="D53" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2904,13 +2947,16 @@
         <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C54" t="s">
-        <v>382</v>
+        <v>207</v>
       </c>
       <c r="D54" t="s">
-        <v>383</v>
+        <v>161</v>
+      </c>
+      <c r="E54" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2918,13 +2964,13 @@
         <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C55" t="s">
-        <v>226</v>
-      </c>
-      <c r="F55" t="s">
-        <v>227</v>
+        <v>214</v>
+      </c>
+      <c r="D55" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -2932,13 +2978,13 @@
         <v>109</v>
       </c>
       <c r="B56" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="C56" t="s">
-        <v>419</v>
+        <v>379</v>
       </c>
       <c r="D56" t="s">
-        <v>420</v>
+        <v>380</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2946,13 +2992,13 @@
         <v>109</v>
       </c>
       <c r="B57" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C57" t="s">
-        <v>421</v>
-      </c>
-      <c r="D57" t="s">
-        <v>420</v>
+        <v>225</v>
+      </c>
+      <c r="F57" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2960,10 +3006,13 @@
         <v>109</v>
       </c>
       <c r="B58" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="C58" t="s">
-        <v>250</v>
+        <v>416</v>
+      </c>
+      <c r="D58" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -2971,13 +3020,13 @@
         <v>109</v>
       </c>
       <c r="B59" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="C59" t="s">
-        <v>252</v>
+        <v>418</v>
       </c>
       <c r="D59" t="s">
-        <v>242</v>
+        <v>417</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2985,13 +3034,10 @@
         <v>109</v>
       </c>
       <c r="B60" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C60" t="s">
-        <v>253</v>
-      </c>
-      <c r="D60" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -2999,13 +3045,13 @@
         <v>109</v>
       </c>
       <c r="B61" t="s">
+        <v>250</v>
+      </c>
+      <c r="C61" t="s">
         <v>251</v>
       </c>
-      <c r="C61" t="s">
-        <v>255</v>
-      </c>
       <c r="D61" t="s">
-        <v>22</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -3013,10 +3059,10 @@
         <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C62" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D62" t="s">
         <v>65</v>
@@ -3030,10 +3076,10 @@
         <v>28</v>
       </c>
       <c r="C63" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D63" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -3044,10 +3090,10 @@
         <v>28</v>
       </c>
       <c r="C64" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D64" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -3055,13 +3101,13 @@
         <v>109</v>
       </c>
       <c r="B65" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C65" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D65" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -3069,10 +3115,10 @@
         <v>109</v>
       </c>
       <c r="B66" t="s">
-        <v>249</v>
+        <v>434</v>
       </c>
       <c r="C66" t="s">
-        <v>259</v>
+        <v>435</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -3080,13 +3126,13 @@
         <v>109</v>
       </c>
       <c r="B67" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C67" t="s">
-        <v>260</v>
+        <v>436</v>
       </c>
       <c r="D67" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -3094,13 +3140,13 @@
         <v>109</v>
       </c>
       <c r="B68" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C68" t="s">
-        <v>261</v>
+        <v>437</v>
       </c>
       <c r="D68" t="s">
-        <v>244</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -3108,10 +3154,10 @@
         <v>109</v>
       </c>
       <c r="B69" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C69" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -3119,13 +3165,13 @@
         <v>109</v>
       </c>
       <c r="B70" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C70" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D70" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -3133,13 +3179,13 @@
         <v>109</v>
       </c>
       <c r="B71" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C71" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D71" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -3147,13 +3193,10 @@
         <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C72" t="s">
-        <v>264</v>
-      </c>
-      <c r="D72" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -3161,13 +3204,13 @@
         <v>109</v>
       </c>
       <c r="B73" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C73" t="s">
+        <v>264</v>
+      </c>
+      <c r="D73" t="s">
         <v>265</v>
-      </c>
-      <c r="D73" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -3175,13 +3218,13 @@
         <v>109</v>
       </c>
       <c r="B74" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C74" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D74" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -3189,13 +3232,13 @@
         <v>109</v>
       </c>
       <c r="B75" t="s">
-        <v>28</v>
+        <v>250</v>
       </c>
       <c r="C75" t="s">
-        <v>427</v>
+        <v>261</v>
       </c>
       <c r="D75" t="s">
-        <v>428</v>
+        <v>241</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -3203,13 +3246,13 @@
         <v>109</v>
       </c>
       <c r="B76" t="s">
-        <v>425</v>
+        <v>250</v>
       </c>
       <c r="C76" t="s">
-        <v>426</v>
+        <v>262</v>
       </c>
       <c r="D76" t="s">
-        <v>420</v>
+        <v>243</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -3217,10 +3260,13 @@
         <v>109</v>
       </c>
       <c r="B77" t="s">
-        <v>397</v>
+        <v>250</v>
       </c>
       <c r="C77" t="s">
-        <v>381</v>
+        <v>263</v>
+      </c>
+      <c r="D77" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -3228,13 +3274,13 @@
         <v>109</v>
       </c>
       <c r="B78" t="s">
-        <v>230</v>
+        <v>28</v>
       </c>
       <c r="C78" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D78" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -3242,10 +3288,13 @@
         <v>109</v>
       </c>
       <c r="B79" t="s">
-        <v>361</v>
+        <v>422</v>
       </c>
       <c r="C79" t="s">
-        <v>398</v>
+        <v>423</v>
+      </c>
+      <c r="D79" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -3253,13 +3302,10 @@
         <v>109</v>
       </c>
       <c r="B80" t="s">
-        <v>363</v>
+        <v>444</v>
       </c>
       <c r="C80" t="s">
-        <v>399</v>
-      </c>
-      <c r="D80" t="s">
-        <v>400</v>
+        <v>440</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -3267,13 +3313,10 @@
         <v>109</v>
       </c>
       <c r="B81" t="s">
-        <v>363</v>
+        <v>444</v>
       </c>
       <c r="C81" t="s">
-        <v>401</v>
-      </c>
-      <c r="D81" t="s">
-        <v>402</v>
+        <v>441</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -3281,91 +3324,91 @@
         <v>109</v>
       </c>
       <c r="B82" t="s">
-        <v>230</v>
+        <v>445</v>
       </c>
       <c r="C82" t="s">
-        <v>424</v>
+        <v>446</v>
       </c>
       <c r="D82" t="s">
-        <v>420</v>
+        <v>435</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B83" t="s">
-        <v>249</v>
+        <v>394</v>
       </c>
       <c r="C83" t="s">
-        <v>278</v>
+        <v>378</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B84" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="C84" t="s">
-        <v>279</v>
+        <v>420</v>
       </c>
       <c r="D84" t="s">
-        <v>280</v>
+        <v>417</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B85" t="s">
-        <v>70</v>
+        <v>358</v>
       </c>
       <c r="C85" t="s">
-        <v>281</v>
-      </c>
-      <c r="D85" t="s">
-        <v>282</v>
+        <v>395</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B86" t="s">
-        <v>70</v>
+        <v>360</v>
       </c>
       <c r="C86" t="s">
-        <v>283</v>
+        <v>396</v>
       </c>
       <c r="D86" t="s">
-        <v>284</v>
+        <v>397</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B87" t="s">
-        <v>285</v>
+        <v>360</v>
       </c>
       <c r="C87" t="s">
-        <v>286</v>
+        <v>398</v>
+      </c>
+      <c r="D87" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="C88" t="s">
-        <v>287</v>
+        <v>421</v>
       </c>
       <c r="D88" t="s">
-        <v>288</v>
+        <v>417</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -3373,10 +3416,10 @@
         <v>104</v>
       </c>
       <c r="B89" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C89" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -3384,13 +3427,13 @@
         <v>104</v>
       </c>
       <c r="B90" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C90" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="D90" t="s">
-        <v>242</v>
+        <v>277</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -3398,13 +3441,13 @@
         <v>104</v>
       </c>
       <c r="B91" t="s">
-        <v>251</v>
+        <v>70</v>
       </c>
       <c r="C91" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="D91" t="s">
-        <v>242</v>
+        <v>279</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -3412,10 +3455,13 @@
         <v>104</v>
       </c>
       <c r="B92" t="s">
-        <v>249</v>
+        <v>70</v>
       </c>
       <c r="C92" t="s">
-        <v>294</v>
+        <v>280</v>
+      </c>
+      <c r="D92" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -3423,13 +3469,10 @@
         <v>104</v>
       </c>
       <c r="B93" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="C93" t="s">
-        <v>295</v>
-      </c>
-      <c r="D93" t="s">
-        <v>242</v>
+        <v>283</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -3437,13 +3480,13 @@
         <v>104</v>
       </c>
       <c r="B94" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C94" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="D94" t="s">
-        <v>242</v>
+        <v>285</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -3451,13 +3494,10 @@
         <v>104</v>
       </c>
       <c r="B95" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C95" t="s">
-        <v>297</v>
-      </c>
-      <c r="D95" t="s">
-        <v>242</v>
+        <v>286</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -3465,13 +3505,13 @@
         <v>104</v>
       </c>
       <c r="B96" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C96" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="D96" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -3479,13 +3519,13 @@
         <v>104</v>
       </c>
       <c r="B97" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C97" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="D97" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -3493,13 +3533,10 @@
         <v>104</v>
       </c>
       <c r="B98" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C98" t="s">
-        <v>300</v>
-      </c>
-      <c r="D98" t="s">
-        <v>242</v>
+        <v>291</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -3507,10 +3544,13 @@
         <v>104</v>
       </c>
       <c r="B99" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C99" t="s">
-        <v>301</v>
+        <v>292</v>
+      </c>
+      <c r="D99" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -3518,13 +3558,13 @@
         <v>104</v>
       </c>
       <c r="B100" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C100" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D100" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -3532,10 +3572,13 @@
         <v>104</v>
       </c>
       <c r="B101" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C101" t="s">
-        <v>303</v>
+        <v>294</v>
+      </c>
+      <c r="D101" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -3543,13 +3586,13 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C102" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="D102" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -3557,13 +3600,13 @@
         <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C103" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D103" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -3571,10 +3614,13 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C104" t="s">
-        <v>306</v>
+        <v>297</v>
+      </c>
+      <c r="D104" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -3582,13 +3628,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C105" t="s">
-        <v>307</v>
-      </c>
-      <c r="D105" t="s">
-        <v>242</v>
+        <v>298</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -3596,13 +3639,13 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C106" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D106" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -3610,10 +3653,10 @@
         <v>104</v>
       </c>
       <c r="B107" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C107" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -3621,13 +3664,13 @@
         <v>104</v>
       </c>
       <c r="B108" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C108" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D108" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -3635,10 +3678,13 @@
         <v>104</v>
       </c>
       <c r="B109" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C109" t="s">
-        <v>311</v>
+        <v>302</v>
+      </c>
+      <c r="D109" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -3646,13 +3692,10 @@
         <v>104</v>
       </c>
       <c r="B110" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C110" t="s">
-        <v>312</v>
-      </c>
-      <c r="D110" t="s">
-        <v>242</v>
+        <v>303</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -3660,10 +3703,13 @@
         <v>104</v>
       </c>
       <c r="B111" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C111" t="s">
-        <v>313</v>
+        <v>304</v>
+      </c>
+      <c r="D111" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -3671,13 +3717,13 @@
         <v>104</v>
       </c>
       <c r="B112" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C112" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="D112" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
@@ -3685,13 +3731,10 @@
         <v>104</v>
       </c>
       <c r="B113" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C113" t="s">
-        <v>315</v>
-      </c>
-      <c r="D113" t="s">
-        <v>242</v>
+        <v>306</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -3699,13 +3742,13 @@
         <v>104</v>
       </c>
       <c r="B114" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C114" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="D114" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -3713,13 +3756,10 @@
         <v>104</v>
       </c>
       <c r="B115" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C115" t="s">
-        <v>317</v>
-      </c>
-      <c r="D115" t="s">
-        <v>242</v>
+        <v>308</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -3727,10 +3767,13 @@
         <v>104</v>
       </c>
       <c r="B116" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C116" t="s">
-        <v>318</v>
+        <v>309</v>
+      </c>
+      <c r="D116" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -3738,13 +3781,10 @@
         <v>104</v>
       </c>
       <c r="B117" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C117" t="s">
-        <v>319</v>
-      </c>
-      <c r="D117" t="s">
-        <v>242</v>
+        <v>310</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -3752,13 +3792,13 @@
         <v>104</v>
       </c>
       <c r="B118" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C118" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="D118" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -3766,13 +3806,13 @@
         <v>104</v>
       </c>
       <c r="B119" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C119" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D119" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -3780,13 +3820,13 @@
         <v>104</v>
       </c>
       <c r="B120" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C120" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="D120" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -3794,13 +3834,94 @@
         <v>104</v>
       </c>
       <c r="B121" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C121" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="D121" t="s">
-        <v>242</v>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>104</v>
+      </c>
+      <c r="B122" t="s">
+        <v>248</v>
+      </c>
+      <c r="C122" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>104</v>
+      </c>
+      <c r="B123" t="s">
+        <v>250</v>
+      </c>
+      <c r="C123" t="s">
+        <v>316</v>
+      </c>
+      <c r="D123" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>104</v>
+      </c>
+      <c r="B124" t="s">
+        <v>250</v>
+      </c>
+      <c r="C124" t="s">
+        <v>317</v>
+      </c>
+      <c r="D124" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>104</v>
+      </c>
+      <c r="B125" t="s">
+        <v>250</v>
+      </c>
+      <c r="C125" t="s">
+        <v>318</v>
+      </c>
+      <c r="D125" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>104</v>
+      </c>
+      <c r="B126" t="s">
+        <v>250</v>
+      </c>
+      <c r="C126" t="s">
+        <v>319</v>
+      </c>
+      <c r="D126" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>104</v>
+      </c>
+      <c r="B127" t="s">
+        <v>250</v>
+      </c>
+      <c r="C127" t="s">
+        <v>320</v>
+      </c>
+      <c r="D127" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -4419,13 +4540,13 @@
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D39" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F39" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -4436,13 +4557,13 @@
         <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D40" t="s">
         <v>43</v>
       </c>
       <c r="F40" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -4453,13 +4574,13 @@
         <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D41" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F41" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -4470,13 +4591,13 @@
         <v>28</v>
       </c>
       <c r="C42" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D42" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F42" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -4487,13 +4608,13 @@
         <v>28</v>
       </c>
       <c r="C43" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D43" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F43" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -4538,10 +4659,10 @@
         <v>28</v>
       </c>
       <c r="C46" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D46" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -4552,7 +4673,7 @@
         <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D47" t="s">
         <v>49</v>
@@ -4566,13 +4687,13 @@
         <v>109</v>
       </c>
       <c r="B48" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C48" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -4580,10 +4701,10 @@
         <v>109</v>
       </c>
       <c r="B49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D49" t="s">
         <v>72</v>
@@ -4594,13 +4715,13 @@
         <v>109</v>
       </c>
       <c r="B50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D50" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -4608,13 +4729,13 @@
         <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -4622,13 +4743,13 @@
         <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C52" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" t="s">
         <v>172</v>
-      </c>
-      <c r="D52" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -4639,7 +4760,7 @@
         <v>28</v>
       </c>
       <c r="C53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D53" t="s">
         <v>111</v>
@@ -4653,7 +4774,7 @@
         <v>28</v>
       </c>
       <c r="C54" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D54" t="s">
         <v>111</v>
@@ -4667,13 +4788,13 @@
         <v>28</v>
       </c>
       <c r="C55" t="s">
+        <v>190</v>
+      </c>
+      <c r="D55" t="s">
         <v>191</v>
       </c>
-      <c r="D55" t="s">
+      <c r="F55" t="s">
         <v>192</v>
-      </c>
-      <c r="F55" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -4687,7 +4808,7 @@
         <v>129</v>
       </c>
       <c r="F56" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -4698,7 +4819,7 @@
         <v>28</v>
       </c>
       <c r="C57" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D57" t="s">
         <v>51</v>
@@ -4712,7 +4833,7 @@
         <v>28</v>
       </c>
       <c r="C58" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D58" t="s">
         <v>51</v>
@@ -4726,7 +4847,7 @@
         <v>28</v>
       </c>
       <c r="C59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D59" t="s">
         <v>51</v>
@@ -4740,7 +4861,7 @@
         <v>28</v>
       </c>
       <c r="C60" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D60" t="s">
         <v>51</v>
@@ -4754,7 +4875,7 @@
         <v>28</v>
       </c>
       <c r="C61" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D61" t="s">
         <v>51</v>
@@ -4768,7 +4889,7 @@
         <v>28</v>
       </c>
       <c r="C62" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D62" t="s">
         <v>51</v>
@@ -4779,16 +4900,16 @@
         <v>109</v>
       </c>
       <c r="B63" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C63" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D63" t="s">
         <v>111</v>
       </c>
       <c r="F63" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -4796,16 +4917,16 @@
         <v>109</v>
       </c>
       <c r="B64" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D64" t="s">
         <v>111</v>
       </c>
       <c r="F64" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -4816,13 +4937,13 @@
         <v>28</v>
       </c>
       <c r="C65" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D65" t="s">
         <v>27</v>
       </c>
       <c r="F65" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -4833,13 +4954,13 @@
         <v>28</v>
       </c>
       <c r="C66" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D66" t="s">
         <v>96</v>
       </c>
       <c r="F66" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -4847,13 +4968,13 @@
         <v>109</v>
       </c>
       <c r="B67" t="s">
+        <v>216</v>
+      </c>
+      <c r="C67" t="s">
         <v>217</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>218</v>
-      </c>
-      <c r="D67" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -4861,10 +4982,10 @@
         <v>109</v>
       </c>
       <c r="B68" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C68" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D68" t="s">
         <v>111</v>
@@ -4878,13 +4999,13 @@
         <v>28</v>
       </c>
       <c r="C69" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D69" t="s">
         <v>96</v>
       </c>
       <c r="F69" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -4892,10 +5013,10 @@
         <v>109</v>
       </c>
       <c r="B70" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C70" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D70" t="s">
         <v>51</v>
@@ -4906,10 +5027,10 @@
         <v>109</v>
       </c>
       <c r="B71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C71" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D71" t="s">
         <v>27</v>
@@ -4923,7 +5044,7 @@
         <v>28</v>
       </c>
       <c r="C72" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D72" t="s">
         <v>47</v>
@@ -4940,13 +5061,13 @@
         <v>28</v>
       </c>
       <c r="C73" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D73" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F73" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -4957,10 +5078,10 @@
         <v>28</v>
       </c>
       <c r="C74" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D74" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -4971,10 +5092,10 @@
         <v>28</v>
       </c>
       <c r="C75" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D75" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -4985,13 +5106,13 @@
         <v>28</v>
       </c>
       <c r="C76" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D76" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F76" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -4999,10 +5120,10 @@
         <v>109</v>
       </c>
       <c r="B77" t="s">
+        <v>229</v>
+      </c>
+      <c r="C77" t="s">
         <v>230</v>
-      </c>
-      <c r="C77" t="s">
-        <v>231</v>
       </c>
       <c r="D77" t="s">
         <v>51</v>
@@ -5013,10 +5134,10 @@
         <v>109</v>
       </c>
       <c r="B78" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C78" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D78" t="s">
         <v>51</v>
@@ -5027,10 +5148,10 @@
         <v>109</v>
       </c>
       <c r="B79" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C79" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D79" t="s">
         <v>51</v>
@@ -5041,16 +5162,16 @@
         <v>109</v>
       </c>
       <c r="B80" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C80" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D80" t="s">
         <v>51</v>
       </c>
       <c r="F80" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -5058,16 +5179,16 @@
         <v>109</v>
       </c>
       <c r="B81" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C81" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D81" t="s">
         <v>51</v>
       </c>
       <c r="F81" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -5075,16 +5196,16 @@
         <v>109</v>
       </c>
       <c r="B82" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C82" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D82" t="s">
         <v>51</v>
       </c>
       <c r="F82" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -5092,10 +5213,10 @@
         <v>109</v>
       </c>
       <c r="B83" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C83" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D83" t="s">
         <v>51</v>
@@ -5106,13 +5227,13 @@
         <v>109</v>
       </c>
       <c r="B84" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C84" t="s">
+        <v>242</v>
+      </c>
+      <c r="D84" t="s">
         <v>243</v>
-      </c>
-      <c r="D84" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -5120,13 +5241,13 @@
         <v>109</v>
       </c>
       <c r="B85" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C85" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D85" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -5134,10 +5255,10 @@
         <v>109</v>
       </c>
       <c r="B86" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C86" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D86" t="s">
         <v>51</v>
@@ -5148,10 +5269,10 @@
         <v>109</v>
       </c>
       <c r="B87" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C87" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D87" t="s">
         <v>51</v>
@@ -5162,13 +5283,13 @@
         <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C88" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F88" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -5176,16 +5297,16 @@
         <v>109</v>
       </c>
       <c r="B89" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C89" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D89" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F89" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -5193,16 +5314,16 @@
         <v>109</v>
       </c>
       <c r="B90" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C90" t="s">
+        <v>407</v>
+      </c>
+      <c r="D90" t="s">
         <v>410</v>
       </c>
-      <c r="D90" t="s">
-        <v>413</v>
-      </c>
       <c r="F90" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -5210,16 +5331,16 @@
         <v>109</v>
       </c>
       <c r="B91" t="s">
+        <v>406</v>
+      </c>
+      <c r="C91" t="s">
         <v>409</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
+        <v>411</v>
+      </c>
+      <c r="F91" t="s">
         <v>412</v>
-      </c>
-      <c r="D91" t="s">
-        <v>414</v>
-      </c>
-      <c r="F91" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -5227,13 +5348,13 @@
         <v>104</v>
       </c>
       <c r="B92" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C92" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F92" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -5241,10 +5362,10 @@
         <v>104</v>
       </c>
       <c r="B93" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C93" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -5252,13 +5373,13 @@
         <v>104</v>
       </c>
       <c r="B94" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C94" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D94" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -5266,13 +5387,13 @@
         <v>104</v>
       </c>
       <c r="B95" t="s">
+        <v>324</v>
+      </c>
+      <c r="C95" t="s">
         <v>327</v>
       </c>
-      <c r="C95" t="s">
-        <v>330</v>
-      </c>
       <c r="D95" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -5280,16 +5401,16 @@
         <v>104</v>
       </c>
       <c r="B96" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C96" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D96" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F96" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -5297,13 +5418,13 @@
         <v>104</v>
       </c>
       <c r="B97" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C97" t="s">
+        <v>332</v>
+      </c>
+      <c r="D97" t="s">
         <v>335</v>
-      </c>
-      <c r="D97" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -5311,16 +5432,16 @@
         <v>104</v>
       </c>
       <c r="B98" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C98" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D98" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F98" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -5328,13 +5449,13 @@
         <v>104</v>
       </c>
       <c r="B99" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C99" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D99" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -5342,16 +5463,16 @@
         <v>104</v>
       </c>
       <c r="B100" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C100" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D100" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F100" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -5359,13 +5480,13 @@
         <v>104</v>
       </c>
       <c r="B101" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C101" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D101" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -5373,16 +5494,16 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C102" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D102" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F102" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -5393,10 +5514,10 @@
         <v>70</v>
       </c>
       <c r="C103" t="s">
+        <v>342</v>
+      </c>
+      <c r="D103" t="s">
         <v>345</v>
-      </c>
-      <c r="D103" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -5407,10 +5528,10 @@
         <v>70</v>
       </c>
       <c r="C104" t="s">
+        <v>343</v>
+      </c>
+      <c r="D104" t="s">
         <v>346</v>
-      </c>
-      <c r="D104" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -5421,10 +5542,10 @@
         <v>70</v>
       </c>
       <c r="C105" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D105" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -5432,16 +5553,16 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C106" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D106" t="s">
         <v>65</v>
       </c>
       <c r="F106" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -5452,10 +5573,10 @@
         <v>70</v>
       </c>
       <c r="C107" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D107" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -5466,10 +5587,10 @@
         <v>70</v>
       </c>
       <c r="C108" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D108" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -5694,13 +5815,13 @@
         <v>28</v>
       </c>
       <c r="C11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D11" t="s">
         <v>177</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
         <v>178</v>
-      </c>
-      <c r="G11" t="s">
-        <v>179</v>
       </c>
       <c r="H11" t="s">
         <v>129</v>
@@ -5714,13 +5835,13 @@
         <v>28</v>
       </c>
       <c r="C12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" t="s">
         <v>184</v>
       </c>
-      <c r="D12" t="s">
-        <v>185</v>
-      </c>
       <c r="G12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -5731,16 +5852,16 @@
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D13" t="s">
+        <v>185</v>
+      </c>
+      <c r="G13" t="s">
         <v>186</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>187</v>
-      </c>
-      <c r="H13" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -5748,16 +5869,16 @@
         <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C14" t="s">
+        <v>208</v>
+      </c>
+      <c r="D14" t="s">
+        <v>389</v>
+      </c>
+      <c r="H14" t="s">
         <v>209</v>
-      </c>
-      <c r="D14" t="s">
-        <v>392</v>
-      </c>
-      <c r="H14" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -5765,16 +5886,16 @@
         <v>109</v>
       </c>
       <c r="B15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D15" t="s">
+        <v>390</v>
+      </c>
+      <c r="H15" t="s">
         <v>211</v>
-      </c>
-      <c r="D15" t="s">
-        <v>393</v>
-      </c>
-      <c r="H15" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -5782,13 +5903,13 @@
         <v>109</v>
       </c>
       <c r="B16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -5796,10 +5917,10 @@
         <v>109</v>
       </c>
       <c r="B17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F17" t="s">
         <v>104</v>
@@ -5810,27 +5931,27 @@
         <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C18" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G18" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C19" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D19" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F19" t="s">
         <v>104</v>
@@ -5838,36 +5959,36 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>266</v>
+      </c>
+      <c r="B20" t="s">
         <v>269</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>270</v>
+      </c>
+      <c r="D20" t="s">
+        <v>271</v>
+      </c>
+      <c r="F20" t="s">
+        <v>104</v>
+      </c>
+      <c r="H20" t="s">
         <v>272</v>
-      </c>
-      <c r="C20" t="s">
-        <v>273</v>
-      </c>
-      <c r="D20" t="s">
-        <v>274</v>
-      </c>
-      <c r="F20" t="s">
-        <v>104</v>
-      </c>
-      <c r="H20" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C21" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G21" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>